<commit_message>
Moved report to docs
</commit_message>
<xml_diff>
--- a/WBS.xlsx
+++ b/WBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\TA and tutors\briefing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce4214081fea2f0e/Desktop/NTU/Y1/SEM2/SC2002/Assignment/sc2002-bee-tee-ohh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DFEA9F-0F37-4332-9CAF-96E13A6E7389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{22DFEA9F-0F37-4332-9CAF-96E13A6E7389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6821E1A1-3EAA-4F87-A2B9-1DC791A75BD4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">                      Tasks                                 Team Member</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Issue Tracking</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>* Project Manager</t>
   </si>
   <si>
@@ -107,13 +104,28 @@
   </si>
   <si>
     <t>Sequence Diagram</t>
+  </si>
+  <si>
+    <t>*Timmanee Yannaputt</t>
+  </si>
+  <si>
+    <t>Tan Wei Xin</t>
+  </si>
+  <si>
+    <t>Ma Shiqi</t>
+  </si>
+  <si>
+    <t>Koh Kai Jie</t>
+  </si>
+  <si>
+    <t>Ong Jee Shen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +181,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -214,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -255,19 +273,6 @@
       </diagonal>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -329,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,9 +355,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -362,10 +366,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,6 +385,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CB27"/>
+  <dimension ref="A1:CB24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,26 +691,26 @@
     <col min="7" max="7" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="17" max="17" width="36.21875" customWidth="1"/>
+    <col min="17" max="17" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:80" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:80" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -716,26 +724,26 @@
     </row>
     <row r="5" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:80" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:80" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
     </row>
     <row r="7" spans="1:80" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
@@ -744,10 +752,10 @@
         <v>2</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -760,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -828,7 +836,7 @@
     </row>
     <row r="8" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -845,13 +853,15 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="23">
+      <c r="Q8" s="22">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="24"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -866,12 +876,14 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="23">
+      <c r="Q9" s="22">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -887,12 +899,14 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="23">
+      <c r="Q10" s="22">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -908,12 +922,14 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="23">
+      <c r="Q11" s="22">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:80" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -929,161 +945,104 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="23">
+      <c r="Q12" s="22">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+    <row r="13" spans="1:80" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="13">
+        <f>SUM(B8:B12)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13">
+        <f>SUM(D8:D12)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="13">
+        <f>SUM(E8:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <f>SUM(F8:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <f>SUM(G8:G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <f>SUM(H8:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <f>SUM(I8:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <f>SUM(J8:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <f>SUM(K8:K12)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
+        <f>SUM(L8:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="21"/>
       <c r="Q13" s="23"/>
     </row>
-    <row r="14" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="23"/>
-    </row>
-    <row r="15" spans="1:80" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="24"/>
-    </row>
-    <row r="16" spans="1:80" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="14">
-        <f>SUM(B8:B15)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14">
-        <f t="shared" ref="D16:L16" si="0">SUM(D8:D15)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="25"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:80" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:80" x14ac:dyDescent="0.3">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>21</v>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>